<commit_message>
update bad word detector , making it take the words from the excel file and making the admin adding the words in there as welll
</commit_message>
<xml_diff>
--- a/API/Reports/ValidatedContractsReport.xlsx
+++ b/API/Reports/ValidatedContractsReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>RC, INC</t>
-  </si>
-  <si>
-    <t>RC</t>
   </si>
 </sst>
 </file>
@@ -159,7 +156,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -396,56 +393,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0">
-        <v>22</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="0">
-        <v>350</v>
-      </c>
-      <c r="F5" s="0">
-        <v>7</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="0">
-        <v>4</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="0">
-        <v>5</v>
-      </c>
-      <c r="N5" s="0">
-        <v>8000</v>
-      </c>
-      <c r="O5" s="0">
-        <v>19000</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="0">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>